<commit_message>
A decent implement which could run without errors, while, might be stuck in the second state in the controller. There might be some mistakes in the rom reading.
</commit_message>
<xml_diff>
--- a/net_port.xlsx
+++ b/net_port.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="60" windowWidth="13995" windowHeight="6705"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="360">
   <si>
     <t>B9</t>
   </si>
@@ -875,13 +875,287 @@
   </si>
   <si>
     <t>flash_data[15]</t>
+  </si>
+  <si>
+    <t>switches[0]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>switches[1]</t>
+  </si>
+  <si>
+    <t>switches[2]</t>
+  </si>
+  <si>
+    <t>switches[3]</t>
+  </si>
+  <si>
+    <t>switches[4]</t>
+  </si>
+  <si>
+    <t>switches[5]</t>
+  </si>
+  <si>
+    <t>switches[6]</t>
+  </si>
+  <si>
+    <t>switches[7]</t>
+  </si>
+  <si>
+    <t>switches[8]</t>
+  </si>
+  <si>
+    <t>switches[9]</t>
+  </si>
+  <si>
+    <t>switches[10]</t>
+  </si>
+  <si>
+    <t>switches[11]</t>
+  </si>
+  <si>
+    <t>switches[12]</t>
+  </si>
+  <si>
+    <t>switches[13]</t>
+  </si>
+  <si>
+    <t>switches[14]</t>
+  </si>
+  <si>
+    <t>LEDS[0]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LEDS[1]</t>
+  </si>
+  <si>
+    <t>LEDS[2]</t>
+  </si>
+  <si>
+    <t>LEDS[3]</t>
+  </si>
+  <si>
+    <t>LEDS[4]</t>
+  </si>
+  <si>
+    <t>LEDS[5]</t>
+  </si>
+  <si>
+    <t>LEDS[6]</t>
+  </si>
+  <si>
+    <t>LEDS[7]</t>
+  </si>
+  <si>
+    <t>LEDS[8]</t>
+  </si>
+  <si>
+    <t>LEDS[9]</t>
+  </si>
+  <si>
+    <t>LEDS[10]</t>
+  </si>
+  <si>
+    <t>LEDS[11]</t>
+  </si>
+  <si>
+    <t>LEDS[12]</t>
+  </si>
+  <si>
+    <t>LEDS[13]</t>
+  </si>
+  <si>
+    <t>LEDS[14]</t>
+  </si>
+  <si>
+    <t>LEDS[15]</t>
+  </si>
+  <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>K2</t>
+  </si>
+  <si>
+    <t>K7</t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>N1</t>
+  </si>
+  <si>
+    <t>N2</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>V3</t>
+  </si>
+  <si>
+    <t>V4</t>
+  </si>
+  <si>
+    <t>U8</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>E10</t>
+  </si>
+  <si>
+    <t>A11</t>
+  </si>
+  <si>
+    <t>B11</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>D11</t>
+  </si>
+  <si>
+    <t>E11</t>
+  </si>
+  <si>
+    <t>F11</t>
+  </si>
+  <si>
+    <t>A12</t>
+  </si>
+  <si>
+    <t>E12</t>
+  </si>
+  <si>
+    <t>F12</t>
+  </si>
+  <si>
+    <t>A13</t>
+  </si>
+  <si>
+    <t>B13</t>
+  </si>
+  <si>
+    <t>D13</t>
+  </si>
+  <si>
+    <t>E13</t>
+  </si>
+  <si>
+    <t>A14</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>E7</t>
+  </si>
+  <si>
+    <t>F7</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>E8</t>
+  </si>
+  <si>
+    <t>F8</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>E9</t>
+  </si>
+  <si>
+    <t>F9</t>
+  </si>
+  <si>
+    <t>G9</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>B10</t>
+  </si>
+  <si>
+    <t>seg7_out_1[0]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>seg7_out_1[1]</t>
+  </si>
+  <si>
+    <t>seg7_out_1[2]</t>
+  </si>
+  <si>
+    <t>seg7_out_1[3]</t>
+  </si>
+  <si>
+    <t>seg7_out_1[4]</t>
+  </si>
+  <si>
+    <t>seg7_out_1[5]</t>
+  </si>
+  <si>
+    <t>seg7_out_1[6]</t>
+  </si>
+  <si>
+    <t>seg7_out_2[0]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>seg7_out_2[1]</t>
+  </si>
+  <si>
+    <t>seg7_out_2[2]</t>
+  </si>
+  <si>
+    <t>seg7_out_2[3]</t>
+  </si>
+  <si>
+    <t>seg7_out_2[4]</t>
+  </si>
+  <si>
+    <t>seg7_out_2[5]</t>
+  </si>
+  <si>
+    <t>seg7_out_2[6]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -912,6 +1186,12 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -972,7 +1252,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1012,9 +1292,36 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1027,7 +1334,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1313,15 +1620,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D132"/>
+  <dimension ref="A1:D176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="F117" sqref="F117"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="D155" sqref="D155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9" style="1"/>
     <col min="4" max="4" width="10.875" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="1"/>
@@ -2492,7 +2799,366 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="14.25" thickTop="1" x14ac:dyDescent="0.15"/>
+    <row r="132" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.15">
+      <c r="A132" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B132" s="13" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A133" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B133" s="14" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A134" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B134" s="14" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A135" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B135" s="14" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A136" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B136" s="14" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A137" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B137" s="14" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A138" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B138" s="14" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A139" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B139" s="14" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A140" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B140" s="14" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A141" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B141" s="14" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A142" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B142" s="14" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A143" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B143" s="14" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A144" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B144" s="14" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A145" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B145" s="14" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A146" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B146" s="14" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.15">
+      <c r="A147" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B147" s="13" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A148" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B148" s="14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A149" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B149" s="14" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A150" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B150" s="14" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A151" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B151" s="14" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A152" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B152" s="14" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A153" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B153" s="14" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A154" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B154" s="15" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.15">
+      <c r="A155" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B155" s="16" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A156" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B156" s="17" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A157" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B157" s="17" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A158" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B158" s="17" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A159" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B159" s="17" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A160" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B160" s="17" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A161" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B161" s="17" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A162" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B162" s="18" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.15">
+      <c r="A163" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B163" s="19" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A164" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B164" s="17" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A165" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B165" s="17" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A166" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B166" s="17" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A167" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B167" s="17" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A168" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B168" s="17" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A169" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="B169" s="20" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.15">
+      <c r="A170" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B170" s="13" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A171" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B171" s="14" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A172" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B172" s="14" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A173" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B173" s="14" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A174" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B174" s="14" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A175" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="B175" s="14" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A176" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B176" s="21" t="s">
+        <v>345</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>